<commit_message>
Update Excel file used in tests as a correct result
</commit_message>
<xml_diff>
--- a/data/simple.xlsx
+++ b/data/simple.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Content" sheetId="2" r:id="rId2"/>
+    <sheet name="Content" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -398,56 +398,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" customWidth="1" width="15.7"/>
-    <col min="2" max="2" customWidth="1" width="45.7"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>yedxtractVersion</v>
-      </c>
-      <c r="B1" t="str">
-        <v>0.1.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>yedFilename</v>
-      </c>
-      <c r="B2" t="str">
-        <v>simple.graphml</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>yedHash</v>
-      </c>
-      <c r="B3" t="str">
-        <v>34b58f264c0096686a93e689c069e0e6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>extractedFields</v>
-      </c>
-      <c r="B4" t="str">
-        <v>{"node":{"configuration":["$","configuration"],"color":["y:Fill","[0]","$","color"],"color2":["y:Fill","[0]","$","color2"]}}</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -761,4 +711,54 @@
     <ignoredError numberStoredAsText="1" sqref="A1:I14"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="15.7"/>
+    <col min="2" max="2" customWidth="1" width="45.7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>yedxtractVersion</v>
+      </c>
+      <c r="B1" t="str">
+        <v>test</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>yedFilename</v>
+      </c>
+      <c r="B2" t="str">
+        <v>simple.graphml</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>yedHash</v>
+      </c>
+      <c r="B3" t="str">
+        <v>34b58f264c0096686a93e689c069e0e6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>extractedFields</v>
+      </c>
+      <c r="B4" t="str">
+        <v>{"node":{"configuration":["$","configuration"],"color":["y:Fill","[0]","$","color"],"color2":["y:Fill","[0]","$","color2"]}}</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>